<commit_message>
added precise and predictive agents
</commit_message>
<xml_diff>
--- a/RedRunner_Jump.xlsx
+++ b/RedRunner_Jump.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1226,11 +1226,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1319067456"/>
-        <c:axId val="-1319987248"/>
+        <c:axId val="-1963829920"/>
+        <c:axId val="-1967726176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1319067456"/>
+        <c:axId val="-1963829920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="11.0"/>
@@ -1289,12 +1289,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1319987248"/>
+        <c:crossAx val="-1967726176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1319987248"/>
+        <c:axId val="-1967726176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5.0"/>
@@ -1353,7 +1353,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1319067456"/>
+        <c:crossAx val="-1963829920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1953,11 +1953,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1319049216"/>
-        <c:axId val="-1319045456"/>
+        <c:axId val="-2005736096"/>
+        <c:axId val="-2005749024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1319049216"/>
+        <c:axId val="-2005736096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2082,12 +2082,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1319045456"/>
+        <c:crossAx val="-2005749024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1319045456"/>
+        <c:axId val="-2005749024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2204,7 +2204,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1319049216"/>
+        <c:crossAx val="-2005736096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2385,7 +2385,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="log"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -2427,10 +2427,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$C$4:$C$52</c:f>
+              <c:f>Sheet3!$C$4:$C$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
                   <c:v>6.626124</c:v>
                 </c:pt>
@@ -2577,16 +2577,19 @@
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>5.866431</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$D$4:$D$52</c:f>
+              <c:f>Sheet3!$D$4:$D$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
                   <c:v>10.56328</c:v>
                 </c:pt>
@@ -2733,6 +2736,9 @@
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>9.523739999999996</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2752,11 +2758,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1319012624"/>
-        <c:axId val="-1319008864"/>
+        <c:axId val="-2006480336"/>
+        <c:axId val="-2006476576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1319012624"/>
+        <c:axId val="-2006480336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2869,12 +2875,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1319008864"/>
+        <c:crossAx val="-2006476576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1319008864"/>
+        <c:axId val="-2006476576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2987,7 +2993,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1319012624"/>
+        <c:crossAx val="-2006480336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3732,11 +3738,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1306249200"/>
-        <c:axId val="-1272330160"/>
+        <c:axId val="-1967692624"/>
+        <c:axId val="-1967688864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1306249200"/>
+        <c:axId val="-1967692624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3849,12 +3855,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1272330160"/>
+        <c:crossAx val="-1967688864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1272330160"/>
+        <c:axId val="-1967688864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="4.5"/>
@@ -3968,7 +3974,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1306249200"/>
+        <c:crossAx val="-1967692624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6272,7 +6278,7 @@
         <xdr:cNvPr id="13" name="Chart 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{01B8C1F1-1AE2-4FE9-958E-F2906ECEBF12}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01B8C1F1-1AE2-4FE9-958E-F2906ECEBF12}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6313,7 +6319,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A88F3419-3875-4395-BC5B-F6ACCAA23344}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A88F3419-3875-4395-BC5B-F6ACCAA23344}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6349,7 +6355,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{93E3DD4C-E43D-4825-85FD-258E556AF405}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93E3DD4C-E43D-4825-85FD-258E556AF405}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6385,7 +6391,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E5445F70-A52F-4449-85F6-C64FD6536608}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5445F70-A52F-4449-85F6-C64FD6536608}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9773,8 +9779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" zoomScale="93" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T31" sqref="T31"/>
+    <sheetView tabSelected="1" topLeftCell="H10" zoomScale="131" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11152,9 +11158,11 @@
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C53">
+        <v>0.1</v>
+      </c>
       <c r="D53">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>